<commit_message>
police bit finalles with 2 fixed window and kalimasta mandir stirrups no. changed
</commit_message>
<xml_diff>
--- a/ofc/estimates/estimate for iron window at police bit/V.xlsx
+++ b/ofc/estimates/estimate for iron window at police bit/V.xlsx
@@ -9,17 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="18" r:id="rId1"/>
-    <sheet name="WCR" sheetId="6" state="hidden" r:id="rId2"/>
+    <sheet name="aluminium" sheetId="19" r:id="rId2"/>
+    <sheet name="structural glazing" sheetId="20" state="hidden" r:id="rId3"/>
+    <sheet name="fixed window" sheetId="21" r:id="rId4"/>
+    <sheet name="upvc dhoka" sheetId="22" r:id="rId5"/>
+    <sheet name="WCR" sheetId="6" state="hidden" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
-    <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="adopted_rate_aggregate_10_20_mm">[1]District_Rate!$L$6</definedName>
@@ -39,10 +43,18 @@
     <definedName name="description_784">[2]Abstract!$B$300</definedName>
     <definedName name="excavator">[1]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[1]Equipment_Rate!$J$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">new!$A$1:$K$50</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">WCR!$A$1:$K$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">aluminium!$A$1:$K$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'fixed window'!$A$1:$K$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">new!$A$1:$K$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'structural glazing'!$A$1:$K$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'upvc dhoka'!$A$1:$K$45</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">WCR!$A$1:$K$30</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">aluminium!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'fixed window'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">new!$1:$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'structural glazing'!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">'upvc dhoka'!$1:$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="5">WCR!$1:$12</definedName>
     <definedName name="skilled">[1]District_Rate!$D$148</definedName>
     <definedName name="skilled_blacksmith">[1]District_Rate!$D$149</definedName>
     <definedName name="unskilled">[1]District_Rate!$D$156</definedName>
@@ -57,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="61">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -298,6 +310,22 @@
   <si>
     <t>-at door</t>
   </si>
+  <si>
+    <t>Providing and fixing 2 or 3 Panel Sliding window of aluminium section in naturally anodized or black anodized/powder coated color, Section size (87*56*1.2 mm) fitted with 5 mm clear glass without fly mesh shutter (Window size 6'*5' or average area 30 Sq. feet per window).</t>
+  </si>
+  <si>
+    <t>Providing and fixing Structural Glazing of aluminum section in  natural or color anodized/powder coated color Section size (60x50+13x1.3 mm) fitted with 5 mm color glass.
+ (average panel area 6.00 Sq.ft.)</t>
+  </si>
+  <si>
+    <t>Providing and fixing fixed window with top fix glass of aluminium section in naturally anodized or black anodized/powder coated color, Section size (87*25+12*1.20 mm) fitted with 5 mm clear glass without fly mesh shutter (Average area 5 Sq. feet per panel).</t>
+  </si>
+  <si>
+    <t>UPVC Casement Window(frame 60*60 mm, sash 60*78mm White Colour With 5mm Glass)</t>
+  </si>
+  <si>
+    <t>UPVC Single Door with full pannel (frame 60*60mm sash 60X100mm White Colour With  Panel)</t>
+  </si>
 </sst>
 </file>
 
@@ -511,7 +539,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -645,26 +673,28 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -675,6 +705,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -698,38 +759,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1342,7 +1376,4012 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection sqref="A1:K45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="156" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>1</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="45">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30">
+        <f>121/3.281</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="31">
+        <f>(1.5+0.333+0.5)/3.281</f>
+        <v>0.7110637000914356</v>
+      </c>
+      <c r="G10" s="40">
+        <f>PRODUCT(C10:F10)</f>
+        <v>15.733991047436215</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="33">
+        <f>0*SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="33">
+        <v>62.02</v>
+      </c>
+      <c r="J11" s="39">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="39">
+        <f>0.13*G11*18426/360</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28">
+        <v>2</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="48" t="str">
+        <f>B10</f>
+        <v>-For roadside drain</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30">
+        <f>D10</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E15" s="31">
+        <f>E10</f>
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="40">
+        <f>PRODUCT(C15:F15)</f>
+        <v>3.3191100274306611</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="33">
+        <f>0*SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="33">
+        <v>4403.5200000000004</v>
+      </c>
+      <c r="J16" s="39">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="39">
+        <f>G16*0.13*(14817.6/5)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
+        <v>3</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="49" t="str">
+        <f>B25</f>
+        <v>-at window</v>
+      </c>
+      <c r="C20" s="29">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30">
+        <f>D15</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E20" s="31">
+        <f>E15</f>
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="40">
+        <f>PRODUCT(C20:F20)</f>
+        <v>1.1063700091435538</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="33">
+        <f>0*SUM(G20:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="52">
+        <v>11126.38</v>
+      </c>
+      <c r="J21" s="39">
+        <f>G21*I21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="51">
+        <f>0.13*G21*((123027.7+6419.1)/15)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
+        <v>1</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="29">
+        <v>3</v>
+      </c>
+      <c r="D25" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G25" s="40">
+        <f>PRODUCT(C25:F25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="29">
+        <v>0</v>
+      </c>
+      <c r="D26" s="30">
+        <f>2.5/3.281</f>
+        <v>0.76196281621456874</v>
+      </c>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31">
+        <f>6.25/3.281</f>
+        <v>1.9049070405364217</v>
+      </c>
+      <c r="G26" s="40">
+        <f t="shared" ref="G26" si="0">C26*0.032163*D26</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="32"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="33">
+        <f>SUM(G25:G26)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27" s="52">
+        <v>2575.34</v>
+      </c>
+      <c r="J27" s="39">
+        <f>G27*I27</f>
+        <v>4306.2041748223701</v>
+      </c>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="51">
+        <f>0.13*G27*((24343.96)/10)</f>
+        <v>529.16927799366852</v>
+      </c>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="51"/>
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28">
+        <v>2</v>
+      </c>
+      <c r="B30" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="29">
+        <v>3</v>
+      </c>
+      <c r="D31" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G31" s="40">
+        <f>PRODUCT(C31:F31)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H31" s="54"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33">
+        <f>SUM(G31:G31)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="52">
+        <v>6997</v>
+      </c>
+      <c r="J32" s="39">
+        <f>G32*I32</f>
+        <v>11699.624364640056</v>
+      </c>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="51">
+        <f>0.13*J32</f>
+        <v>1520.9511674032074</v>
+      </c>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="28"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="1:13" s="1" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="28">
+        <v>3</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="29">
+        <v>1</v>
+      </c>
+      <c r="D36" s="30">
+        <f>2.5/3.281</f>
+        <v>0.76196281621456874</v>
+      </c>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31">
+        <f>6.25/3.281</f>
+        <v>1.9049070405364217</v>
+      </c>
+      <c r="G36" s="40">
+        <f>PRODUCT(C36:F36)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H36" s="54"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="33">
+        <f>SUM(G36:G36)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I37" s="52">
+        <v>8306.7099999999991</v>
+      </c>
+      <c r="J37" s="39">
+        <f>G37*I37</f>
+        <v>12056.926518358958</v>
+      </c>
+      <c r="K37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="51">
+        <f>0.13*J37</f>
+        <v>1567.4004473866646</v>
+      </c>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="31"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="34"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="51"/>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="28">
+        <v>4</v>
+      </c>
+      <c r="B41" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="29">
+        <v>1</v>
+      </c>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="39">
+        <f>PRODUCT(C41:F41)</f>
+        <v>1</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I41" s="33">
+        <v>500</v>
+      </c>
+      <c r="J41" s="8">
+        <f>G41*I41</f>
+        <v>500</v>
+      </c>
+      <c r="K41" s="31"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="4"/>
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8">
+        <f>SUM(J27:J41)</f>
+        <v>32180.275950604926</v>
+      </c>
+      <c r="K43" s="4"/>
+      <c r="M43" s="44"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M44" s="44"/>
+    </row>
+    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" s="65">
+        <f>J43</f>
+        <v>32180.275950604926</v>
+      </c>
+      <c r="D45" s="66"/>
+      <c r="E45" s="15">
+        <v>100</v>
+      </c>
+      <c r="F45" s="19"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="23"/>
+      <c r="M45" s="19"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="68">
+        <v>28500</v>
+      </c>
+      <c r="D46" s="69"/>
+      <c r="E46" s="15"/>
+      <c r="M46" s="44"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="68">
+        <f>C46-C49-C50</f>
+        <v>27075</v>
+      </c>
+      <c r="D47" s="69"/>
+      <c r="E47" s="15">
+        <f>C47/C45*100</f>
+        <v>84.135387905183705</v>
+      </c>
+      <c r="M47" s="44"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="70">
+        <f>C45-C47</f>
+        <v>5105.275950604926</v>
+      </c>
+      <c r="D48" s="70"/>
+      <c r="E48" s="15">
+        <f>100-E47</f>
+        <v>15.864612094816295</v>
+      </c>
+      <c r="M48" s="44"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" s="65">
+        <f>C46*0.03</f>
+        <v>855</v>
+      </c>
+      <c r="D49" s="66"/>
+      <c r="E49" s="15">
+        <v>3</v>
+      </c>
+      <c r="M49" s="44"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="65">
+        <f>C46*0.02</f>
+        <v>570</v>
+      </c>
+      <c r="D50" s="66"/>
+      <c r="E50" s="15">
+        <v>2</v>
+      </c>
+      <c r="M50" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:    
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M49"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="156" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>1</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="45">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30">
+        <f>121/3.281</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="31">
+        <f>(1.5+0.333+0.5)/3.281</f>
+        <v>0.7110637000914356</v>
+      </c>
+      <c r="G10" s="40">
+        <f>PRODUCT(C10:F10)</f>
+        <v>15.733991047436215</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="33">
+        <f>0*SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="33">
+        <v>62.02</v>
+      </c>
+      <c r="J11" s="39">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="39">
+        <f>0.13*G11*18426/360</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28">
+        <v>2</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="48" t="str">
+        <f>B10</f>
+        <v>-For roadside drain</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30">
+        <f>D10</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E15" s="31">
+        <f>E10</f>
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="40">
+        <f>PRODUCT(C15:F15)</f>
+        <v>3.3191100274306611</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="33">
+        <f>0*SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="33">
+        <v>4403.5200000000004</v>
+      </c>
+      <c r="J16" s="39">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="39">
+        <f>G16*0.13*(14817.6/5)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
+        <v>3</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="49" t="str">
+        <f>B25</f>
+        <v>-at window</v>
+      </c>
+      <c r="C20" s="29">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30">
+        <f>D15</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E20" s="31">
+        <f>E15</f>
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="40">
+        <f>PRODUCT(C20:F20)</f>
+        <v>1.1063700091435538</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="33">
+        <f>0*SUM(G20:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="52">
+        <v>11126.38</v>
+      </c>
+      <c r="J21" s="39">
+        <f>G21*I21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="51">
+        <f>0.13*G21*((123027.7+6419.1)/15)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
+        <v>1</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="29">
+        <v>3</v>
+      </c>
+      <c r="D25" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G25" s="40">
+        <f>PRODUCT(C25:F25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="33">
+        <f>SUM(G25:G25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="52">
+        <v>2575.34</v>
+      </c>
+      <c r="J26" s="39">
+        <f>G26*I26</f>
+        <v>4306.2041748223701</v>
+      </c>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="51">
+        <f>0.13*G26*((24343.96)/10)</f>
+        <v>529.16927799366852</v>
+      </c>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
+        <v>2</v>
+      </c>
+      <c r="B29" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="29">
+        <v>3</v>
+      </c>
+      <c r="D30" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G30" s="40">
+        <f>PRODUCT(C30:F30)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H30" s="54"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="33">
+        <f>SUM(G30:G30)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="52">
+        <v>5918</v>
+      </c>
+      <c r="J31" s="39">
+        <f>G31*I31</f>
+        <v>9895.4376146834147</v>
+      </c>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="51">
+        <f>0.13*J31</f>
+        <v>1286.4068899088441</v>
+      </c>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="28">
+        <v>3</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="29">
+        <v>1</v>
+      </c>
+      <c r="D35" s="30">
+        <f>2.5/3.281</f>
+        <v>0.76196281621456874</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31">
+        <f>6.25/3.281</f>
+        <v>1.9049070405364217</v>
+      </c>
+      <c r="G35" s="40">
+        <f>PRODUCT(C35:F35)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H35" s="54"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="33">
+        <f>SUM(G35:G35)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="52">
+        <v>8306.7099999999991</v>
+      </c>
+      <c r="J36" s="39">
+        <f>G36*I36</f>
+        <v>12056.926518358958</v>
+      </c>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="51">
+        <f>0.13*J36</f>
+        <v>1567.4004473866646</v>
+      </c>
+      <c r="K37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="31"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="28">
+        <v>4</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="29">
+        <v>1</v>
+      </c>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="39">
+        <f>PRODUCT(C40:F40)</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" s="33">
+        <v>500</v>
+      </c>
+      <c r="J40" s="8">
+        <f>G40*I40</f>
+        <v>500</v>
+      </c>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="4"/>
+      <c r="M41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8">
+        <f>SUM(J26:J40)</f>
+        <v>30141.544923153921</v>
+      </c>
+      <c r="K42" s="4"/>
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="44"/>
+    </row>
+    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="65">
+        <f>J42</f>
+        <v>30141.544923153921</v>
+      </c>
+      <c r="D44" s="66"/>
+      <c r="E44" s="15">
+        <v>100</v>
+      </c>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="23"/>
+      <c r="M44" s="19"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="68">
+        <v>26500</v>
+      </c>
+      <c r="D45" s="69"/>
+      <c r="E45" s="15"/>
+      <c r="M45" s="44"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="68">
+        <f>C45-C48-C49</f>
+        <v>25175</v>
+      </c>
+      <c r="D46" s="69"/>
+      <c r="E46" s="15">
+        <f>C46/C44*100</f>
+        <v>83.522593364685989</v>
+      </c>
+      <c r="M46" s="44"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="70">
+        <f>C44-C46</f>
+        <v>4966.5449231539205</v>
+      </c>
+      <c r="D47" s="70"/>
+      <c r="E47" s="15">
+        <f>100-E46</f>
+        <v>16.477406635314011</v>
+      </c>
+      <c r="M47" s="44"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="65">
+        <f>C45*0.03</f>
+        <v>795</v>
+      </c>
+      <c r="D48" s="66"/>
+      <c r="E48" s="15">
+        <v>3</v>
+      </c>
+      <c r="M48" s="44"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="65">
+        <f>C45*0.02</f>
+        <v>530</v>
+      </c>
+      <c r="D49" s="66"/>
+      <c r="E49" s="15">
+        <v>2</v>
+      </c>
+      <c r="M49" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:    
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="156" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>1</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="45">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30">
+        <f>121/3.281</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="31">
+        <f>(1.5+0.333+0.5)/3.281</f>
+        <v>0.7110637000914356</v>
+      </c>
+      <c r="G10" s="40">
+        <f>PRODUCT(C10:F10)</f>
+        <v>15.733991047436215</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="33">
+        <f>0*SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="33">
+        <v>62.02</v>
+      </c>
+      <c r="J11" s="39">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="39">
+        <f>0.13*G11*18426/360</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28">
+        <v>2</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="48" t="str">
+        <f>B10</f>
+        <v>-For roadside drain</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30">
+        <f>D10</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E15" s="31">
+        <f>E10</f>
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="40">
+        <f>PRODUCT(C15:F15)</f>
+        <v>3.3191100274306611</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="33">
+        <f>0*SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="33">
+        <v>4403.5200000000004</v>
+      </c>
+      <c r="J16" s="39">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="39">
+        <f>G16*0.13*(14817.6/5)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
+        <v>3</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="49" t="str">
+        <f>B25</f>
+        <v>-at window</v>
+      </c>
+      <c r="C20" s="29">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30">
+        <f>D15</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E20" s="31">
+        <f>E15</f>
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="40">
+        <f>PRODUCT(C20:F20)</f>
+        <v>1.1063700091435538</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="33">
+        <f>0*SUM(G20:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="52">
+        <v>11126.38</v>
+      </c>
+      <c r="J21" s="39">
+        <f>G21*I21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="51">
+        <f>0.13*G21*((123027.7+6419.1)/15)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
+        <v>1</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="29">
+        <v>3</v>
+      </c>
+      <c r="D25" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G25" s="40">
+        <f>PRODUCT(C25:F25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="33">
+        <f>SUM(G25:G25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="52">
+        <v>2575.34</v>
+      </c>
+      <c r="J26" s="39">
+        <f>G26*I26</f>
+        <v>4306.2041748223701</v>
+      </c>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="51">
+        <f>0.13*G26*((24343.96)/10)</f>
+        <v>529.16927799366852</v>
+      </c>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
+        <v>2</v>
+      </c>
+      <c r="B29" s="83" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="29">
+        <v>3</v>
+      </c>
+      <c r="D30" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G30" s="40">
+        <f>PRODUCT(C30:F30)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H30" s="54"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="33">
+        <f>SUM(G30:G30)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="52">
+        <v>6283.84</v>
+      </c>
+      <c r="J31" s="39">
+        <f>G31*I31</f>
+        <v>10507.15557631839</v>
+      </c>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="51">
+        <f>0.13*J31</f>
+        <v>1365.9302249213906</v>
+      </c>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="28">
+        <v>3</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="55"/>
+      <c r="D34" s="55"/>
+      <c r="E34" s="55"/>
+      <c r="F34" s="55"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="55"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="29">
+        <v>1</v>
+      </c>
+      <c r="D35" s="30">
+        <f>2.5/3.281</f>
+        <v>0.76196281621456874</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31">
+        <f>6.25/3.281</f>
+        <v>1.9049070405364217</v>
+      </c>
+      <c r="G35" s="40">
+        <f>PRODUCT(C35:F35)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H35" s="54"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="33">
+        <f>SUM(G35:G35)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="52">
+        <v>8306.7099999999991</v>
+      </c>
+      <c r="J36" s="39">
+        <f>G36*I36</f>
+        <v>12056.926518358958</v>
+      </c>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="51">
+        <f>0.13*J36</f>
+        <v>1567.4004473866646</v>
+      </c>
+      <c r="K37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="34"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="31"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="28">
+        <v>4</v>
+      </c>
+      <c r="B40" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="29">
+        <v>1</v>
+      </c>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="39">
+        <f>PRODUCT(C40:F40)</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I40" s="33">
+        <v>500</v>
+      </c>
+      <c r="J40" s="8">
+        <f>G40*I40</f>
+        <v>500</v>
+      </c>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="4"/>
+      <c r="M41" s="44"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8">
+        <f>SUM(J26:J40)</f>
+        <v>30832.786219801441</v>
+      </c>
+      <c r="K42" s="4"/>
+      <c r="M42" s="44"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M43" s="44"/>
+    </row>
+    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="65">
+        <f>J42</f>
+        <v>30832.786219801441</v>
+      </c>
+      <c r="D44" s="66"/>
+      <c r="E44" s="15">
+        <v>100</v>
+      </c>
+      <c r="F44" s="19"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="23"/>
+      <c r="M44" s="19"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="68">
+        <v>28500</v>
+      </c>
+      <c r="D45" s="69"/>
+      <c r="E45" s="15"/>
+      <c r="M45" s="44"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C46" s="68">
+        <f>C45-C48-C49</f>
+        <v>27075</v>
+      </c>
+      <c r="D46" s="69"/>
+      <c r="E46" s="15">
+        <f>C46/C44*100</f>
+        <v>87.81236897303782</v>
+      </c>
+      <c r="M46" s="44"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B47" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="70">
+        <f>C44-C46</f>
+        <v>3757.7862198014409</v>
+      </c>
+      <c r="D47" s="70"/>
+      <c r="E47" s="15">
+        <f>100-E46</f>
+        <v>12.18763102696218</v>
+      </c>
+      <c r="M47" s="44"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B48" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C48" s="65">
+        <f>C45*0.03</f>
+        <v>855</v>
+      </c>
+      <c r="D48" s="66"/>
+      <c r="E48" s="15">
+        <v>3</v>
+      </c>
+      <c r="M48" s="44"/>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C49" s="65">
+        <f>C45*0.02</f>
+        <v>570</v>
+      </c>
+      <c r="D49" s="66"/>
+      <c r="E49" s="15">
+        <v>2</v>
+      </c>
+      <c r="M49" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:    
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection sqref="A1:K49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="64"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="60" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="156" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28">
+        <v>1</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="31"/>
+    </row>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="45">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30">
+        <f>121/3.281</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E10" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="F10" s="31">
+        <f>(1.5+0.333+0.5)/3.281</f>
+        <v>0.7110637000914356</v>
+      </c>
+      <c r="G10" s="40">
+        <f>PRODUCT(C10:F10)</f>
+        <v>15.733991047436215</v>
+      </c>
+      <c r="H10" s="54"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="33">
+        <f>0*SUM(G10:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="33">
+        <v>62.02</v>
+      </c>
+      <c r="J11" s="39">
+        <f>G11*I11</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="31"/>
+    </row>
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
+      <c r="B12" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="39">
+        <f>0.13*G11*18426/360</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="31"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="28">
+        <v>2</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="31"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="48" t="str">
+        <f>B10</f>
+        <v>-For roadside drain</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30">
+        <f>D10</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E15" s="31">
+        <f>E10</f>
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="40">
+        <f>PRODUCT(C15:F15)</f>
+        <v>3.3191100274306611</v>
+      </c>
+      <c r="H15" s="54"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="31"/>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="33">
+        <f>0*SUM(G15:G15)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="33">
+        <v>4403.5200000000004</v>
+      </c>
+      <c r="J16" s="39">
+        <f>G16*I16</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="31"/>
+    </row>
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="39">
+        <f>G16*0.13*(14817.6/5)</f>
+        <v>0</v>
+      </c>
+      <c r="K17" s="31"/>
+    </row>
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="31"/>
+    </row>
+    <row r="19" spans="1:11" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="28">
+        <v>3</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="31"/>
+    </row>
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28"/>
+      <c r="B20" s="49" t="str">
+        <f>B25</f>
+        <v>-at window</v>
+      </c>
+      <c r="C20" s="29">
+        <v>1</v>
+      </c>
+      <c r="D20" s="30">
+        <f>D15</f>
+        <v>36.879000304785123</v>
+      </c>
+      <c r="E20" s="31">
+        <f>E15</f>
+        <v>0.6</v>
+      </c>
+      <c r="F20" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="40">
+        <f>PRODUCT(C20:F20)</f>
+        <v>1.1063700091435538</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="31"/>
+    </row>
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28"/>
+      <c r="B21" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="33">
+        <f>0*SUM(G20:G20)</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="52">
+        <v>11126.38</v>
+      </c>
+      <c r="J21" s="39">
+        <f>G21*I21</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="31"/>
+    </row>
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="28"/>
+      <c r="B22" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="51">
+        <f>0.13*G21*((123027.7+6419.1)/15)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="31"/>
+    </row>
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="28"/>
+      <c r="B23" s="34"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="31"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="91.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="28">
+        <v>1</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="31"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="28"/>
+      <c r="B25" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="29">
+        <v>3</v>
+      </c>
+      <c r="D25" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G25" s="40">
+        <f>PRODUCT(C25:F25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="31"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="28"/>
+      <c r="B26" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="33">
+        <f>SUM(G25:G25)</f>
+        <v>1.6720915198856734</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I26" s="52">
+        <v>2575.34</v>
+      </c>
+      <c r="J26" s="39">
+        <f>G26*I26</f>
+        <v>4306.2041748223701</v>
+      </c>
+      <c r="K26" s="31"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="51">
+        <f>0.13*G26*((24343.96)/10)</f>
+        <v>529.16927799366852</v>
+      </c>
+      <c r="K27" s="31"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="28"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="51"/>
+      <c r="K28" s="31"/>
+    </row>
+    <row r="29" spans="1:11" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28">
+        <v>2</v>
+      </c>
+      <c r="B29" s="83" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="29"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="31"/>
+    </row>
+    <row r="30" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28"/>
+      <c r="B30" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="29">
+        <v>2</v>
+      </c>
+      <c r="D30" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G30" s="40">
+        <f>PRODUCT(C30:F30)</f>
+        <v>1.1147276799237822</v>
+      </c>
+      <c r="H30" s="54"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="31"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="28"/>
+      <c r="B31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="33">
+        <f>SUM(G30:G30)</f>
+        <v>1.1147276799237822</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="52">
+        <v>4605.28</v>
+      </c>
+      <c r="J31" s="39">
+        <f>G31*I31</f>
+        <v>5133.6330897993957</v>
+      </c>
+      <c r="K31" s="31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="28"/>
+      <c r="B32" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="51">
+        <f>0.13*J31</f>
+        <v>667.37230167392147</v>
+      </c>
+      <c r="K32" s="31"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="28"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="31"/>
+    </row>
+    <row r="34" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="A34" s="28">
+        <v>3</v>
+      </c>
+      <c r="B34" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="31"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="28"/>
+      <c r="B35" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C35" s="29">
+        <v>1</v>
+      </c>
+      <c r="D35" s="30">
+        <f>2/3.281</f>
+        <v>0.6095702529716549</v>
+      </c>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31">
+        <f>3/3.281</f>
+        <v>0.91435537945748246</v>
+      </c>
+      <c r="G35" s="40">
+        <f>PRODUCT(C35:F35)</f>
+        <v>0.55736383996189109</v>
+      </c>
+      <c r="H35" s="54"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="39"/>
+      <c r="K35" s="31"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="28"/>
+      <c r="B36" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="33">
+        <f>SUM(G35:G35)</f>
+        <v>0.55736383996189109</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="52">
+        <v>5918</v>
+      </c>
+      <c r="J36" s="39">
+        <f>G36*I36</f>
+        <v>3298.4792048944714</v>
+      </c>
+      <c r="K36" s="31"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="28"/>
+      <c r="B37" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="32"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="51">
+        <f>0.13*J36</f>
+        <v>428.80229663628131</v>
+      </c>
+      <c r="K37" s="31"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="34"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="32"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="31"/>
+    </row>
+    <row r="39" spans="1:13" s="1" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="28">
+        <v>4</v>
+      </c>
+      <c r="B39" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+      <c r="F39" s="55"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="55"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="31"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="28"/>
+      <c r="B40" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="29">
+        <v>1</v>
+      </c>
+      <c r="D40" s="30">
+        <f>2.5/3.281</f>
+        <v>0.76196281621456874</v>
+      </c>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31">
+        <f>6.25/3.281</f>
+        <v>1.9049070405364217</v>
+      </c>
+      <c r="G40" s="40">
+        <f>PRODUCT(C40:F40)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H40" s="54"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="31"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
+      <c r="B41" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="29"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="33">
+        <f>SUM(G40:G40)</f>
+        <v>1.4514683332340914</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="52">
+        <v>8306.7099999999991</v>
+      </c>
+      <c r="J41" s="39">
+        <f>G41*I41</f>
+        <v>12056.926518358958</v>
+      </c>
+      <c r="K41" s="31"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="28"/>
+      <c r="B42" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="29"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="51">
+        <f>0.13*J41</f>
+        <v>1567.4004473866646</v>
+      </c>
+      <c r="K42" s="31"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="28"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="31"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="28"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="33"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="51"/>
+      <c r="K44" s="31"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="28">
+        <v>5</v>
+      </c>
+      <c r="B45" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="29">
+        <v>1</v>
+      </c>
+      <c r="D45" s="30"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="39">
+        <f>PRODUCT(C45:F45)</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="I45" s="33">
+        <v>500</v>
+      </c>
+      <c r="J45" s="8">
+        <f>G45*I45</f>
+        <v>500</v>
+      </c>
+      <c r="K45" s="31"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="4"/>
+      <c r="M46" s="44"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8">
+        <f>SUM(J26:J45)</f>
+        <v>28487.987311565732</v>
+      </c>
+      <c r="K47" s="4"/>
+      <c r="M47" s="44"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M48" s="44"/>
+    </row>
+    <row r="49" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="65">
+        <f>J47</f>
+        <v>28487.987311565732</v>
+      </c>
+      <c r="D49" s="66"/>
+      <c r="E49" s="15">
+        <v>100</v>
+      </c>
+      <c r="F49" s="19"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="23"/>
+      <c r="M49" s="19"/>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B50" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="68">
+        <v>25000</v>
+      </c>
+      <c r="D50" s="69"/>
+      <c r="E50" s="15"/>
+      <c r="M50" s="44"/>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B51" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="68">
+        <f>C50-C53-C54</f>
+        <v>23750</v>
+      </c>
+      <c r="D51" s="69"/>
+      <c r="E51" s="15">
+        <f>C51/C49*100</f>
+        <v>83.368472964595242</v>
+      </c>
+      <c r="M51" s="44"/>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B52" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C52" s="70">
+        <f>C49-C51</f>
+        <v>4737.9873115657319</v>
+      </c>
+      <c r="D52" s="70"/>
+      <c r="E52" s="15">
+        <f>100-E51</f>
+        <v>16.631527035404758</v>
+      </c>
+      <c r="M52" s="44"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B53" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="65">
+        <f>C50*0.03</f>
+        <v>750</v>
+      </c>
+      <c r="D53" s="66"/>
+      <c r="E53" s="15">
+        <v>3</v>
+      </c>
+      <c r="M53" s="44"/>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B54" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="65">
+        <f>C50*0.02</f>
+        <v>500</v>
+      </c>
+      <c r="D54" s="66"/>
+      <c r="E54" s="15">
+        <v>2</v>
+      </c>
+      <c r="M54" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:    
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
@@ -1441,38 +5480,38 @@
       <c r="K5" s="64"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="56" t="s">
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="56" t="s">
+      <c r="H7" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1496,7 +5535,7 @@
       <c r="G8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="77" t="s">
+      <c r="H8" s="53" t="s">
         <v>12</v>
       </c>
       <c r="I8" s="25" t="s">
@@ -1521,7 +5560,7 @@
       <c r="E9" s="17"/>
       <c r="F9" s="17"/>
       <c r="G9" s="43"/>
-      <c r="H9" s="78"/>
+      <c r="H9" s="54"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
       <c r="K9" s="31"/>
@@ -1549,7 +5588,7 @@
         <f>PRODUCT(C10:F10)</f>
         <v>15.733991047436215</v>
       </c>
-      <c r="H10" s="78"/>
+      <c r="H10" s="54"/>
       <c r="I10" s="33"/>
       <c r="J10" s="33"/>
       <c r="K10" s="31"/>
@@ -1567,7 +5606,7 @@
         <f>0*SUM(G10:G10)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="78" t="s">
+      <c r="H11" s="54" t="s">
         <v>34</v>
       </c>
       <c r="I11" s="33">
@@ -1589,7 +5628,7 @@
       <c r="E12" s="31"/>
       <c r="F12" s="31"/>
       <c r="G12" s="33"/>
-      <c r="H12" s="78"/>
+      <c r="H12" s="54"/>
       <c r="I12" s="33"/>
       <c r="J12" s="39">
         <f>0.13*G11*18426/360</f>
@@ -1605,7 +5644,7 @@
       <c r="E13" s="31"/>
       <c r="F13" s="31"/>
       <c r="G13" s="33"/>
-      <c r="H13" s="78"/>
+      <c r="H13" s="54"/>
       <c r="I13" s="33"/>
       <c r="J13" s="39"/>
       <c r="K13" s="31"/>
@@ -1622,7 +5661,7 @@
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="33"/>
-      <c r="H14" s="78"/>
+      <c r="H14" s="54"/>
       <c r="I14" s="33"/>
       <c r="J14" s="39"/>
       <c r="K14" s="31"/>
@@ -1651,7 +5690,7 @@
         <f>PRODUCT(C15:F15)</f>
         <v>3.3191100274306611</v>
       </c>
-      <c r="H15" s="78"/>
+      <c r="H15" s="54"/>
       <c r="I15" s="33"/>
       <c r="J15" s="39"/>
       <c r="K15" s="31"/>
@@ -1669,7 +5708,7 @@
         <f>0*SUM(G15:G15)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="78" t="s">
+      <c r="H16" s="54" t="s">
         <v>34</v>
       </c>
       <c r="I16" s="33">
@@ -1691,7 +5730,7 @@
       <c r="E17" s="31"/>
       <c r="F17" s="31"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="78"/>
+      <c r="H17" s="54"/>
       <c r="I17" s="33"/>
       <c r="J17" s="39">
         <f>G16*0.13*(14817.6/5)</f>
@@ -1707,7 +5746,7 @@
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="33"/>
-      <c r="H18" s="78"/>
+      <c r="H18" s="54"/>
       <c r="I18" s="33"/>
       <c r="J18" s="39"/>
       <c r="K18" s="31"/>
@@ -1724,7 +5763,7 @@
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
       <c r="G19" s="33"/>
-      <c r="H19" s="78"/>
+      <c r="H19" s="54"/>
       <c r="I19" s="33"/>
       <c r="J19" s="39"/>
       <c r="K19" s="31"/>
@@ -1753,7 +5792,7 @@
         <f>PRODUCT(C20:F20)</f>
         <v>1.1063700091435538</v>
       </c>
-      <c r="H20" s="78"/>
+      <c r="H20" s="54"/>
       <c r="I20" s="33"/>
       <c r="J20" s="39"/>
       <c r="K20" s="31"/>
@@ -1771,7 +5810,7 @@
         <f>0*SUM(G20:G20)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="78" t="s">
+      <c r="H21" s="54" t="s">
         <v>34</v>
       </c>
       <c r="I21" s="52">
@@ -1793,7 +5832,7 @@
       <c r="E22" s="31"/>
       <c r="F22" s="31"/>
       <c r="G22" s="33"/>
-      <c r="H22" s="78"/>
+      <c r="H22" s="54"/>
       <c r="I22" s="33"/>
       <c r="J22" s="51">
         <f>0.13*G21*((123027.7+6419.1)/15)</f>
@@ -1809,7 +5848,7 @@
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="33"/>
-      <c r="H23" s="78"/>
+      <c r="H23" s="54"/>
       <c r="I23" s="33"/>
       <c r="J23" s="51"/>
       <c r="K23" s="31"/>
@@ -1818,15 +5857,15 @@
       <c r="A24" s="28">
         <v>1</v>
       </c>
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80"/>
-      <c r="E24" s="80"/>
-      <c r="F24" s="80"/>
-      <c r="G24" s="80"/>
-      <c r="H24" s="81"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="56"/>
+      <c r="H24" s="57"/>
       <c r="I24" s="33"/>
       <c r="J24" s="39"/>
       <c r="K24" s="31"/>
@@ -1852,7 +5891,7 @@
         <f>PRODUCT(C25:F25)</f>
         <v>1.6720915198856734</v>
       </c>
-      <c r="H25" s="78"/>
+      <c r="H25" s="54"/>
       <c r="I25" s="33"/>
       <c r="J25" s="39"/>
       <c r="K25" s="31"/>
@@ -1939,21 +5978,21 @@
       <c r="J29" s="51"/>
       <c r="K29" s="31"/>
     </row>
-    <row r="30" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>2</v>
       </c>
-      <c r="B30" s="82" t="s">
-        <v>52</v>
+      <c r="B30" s="84" t="s">
+        <v>59</v>
       </c>
       <c r="C30" s="29"/>
       <c r="D30" s="30"/>
       <c r="E30" s="31"/>
       <c r="F30" s="31"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="32"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="54"/>
       <c r="I30" s="33"/>
-      <c r="J30" s="51"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="31"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1977,7 +6016,7 @@
         <f>PRODUCT(C31:F31)</f>
         <v>1.6720915198856734</v>
       </c>
-      <c r="H31" s="78"/>
+      <c r="H31" s="54"/>
       <c r="I31" s="33"/>
       <c r="J31" s="39"/>
       <c r="K31" s="31"/>
@@ -1999,11 +6038,11 @@
         <v>34</v>
       </c>
       <c r="I32" s="52">
-        <v>6997</v>
+        <v>7867</v>
       </c>
       <c r="J32" s="39">
         <f>G32*I32</f>
-        <v>11699.624364640056</v>
+        <v>13154.343986940592</v>
       </c>
       <c r="K32" s="31"/>
     </row>
@@ -2021,7 +6060,7 @@
       <c r="I33" s="33"/>
       <c r="J33" s="51">
         <f>0.13*J32</f>
-        <v>1520.9511674032074</v>
+        <v>1710.064718302277</v>
       </c>
       <c r="K33" s="31"/>
     </row>
@@ -2038,19 +6077,19 @@
       <c r="J34" s="51"/>
       <c r="K34" s="31"/>
     </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" ht="60.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="1" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28">
         <v>3</v>
       </c>
-      <c r="B35" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
+      <c r="B35" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="55"/>
+      <c r="D35" s="55"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="55"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="33"/>
       <c r="J35" s="51"/>
       <c r="K35" s="31"/>
@@ -2076,7 +6115,7 @@
         <f>PRODUCT(C36:F36)</f>
         <v>1.4514683332340914</v>
       </c>
-      <c r="H36" s="78"/>
+      <c r="H36" s="54"/>
       <c r="I36" s="33"/>
       <c r="J36" s="39"/>
       <c r="K36" s="31"/>
@@ -2098,11 +6137,11 @@
         <v>34</v>
       </c>
       <c r="I37" s="52">
-        <v>8306.7099999999991</v>
+        <v>8744</v>
       </c>
       <c r="J37" s="39">
         <f>G37*I37</f>
-        <v>12056.926518358958</v>
+        <v>12691.639105798895</v>
       </c>
       <c r="K37" s="31"/>
     </row>
@@ -2120,7 +6159,7 @@
       <c r="I38" s="33"/>
       <c r="J38" s="51">
         <f>0.13*J37</f>
-        <v>1567.4004473866646</v>
+        <v>1649.9130837538564</v>
       </c>
       <c r="K38" s="31"/>
     </row>
@@ -2207,7 +6246,7 @@
       <c r="I43" s="8"/>
       <c r="J43" s="8">
         <f>SUM(J27:J41)</f>
-        <v>32180.275950604926</v>
+        <v>34541.334347611657</v>
       </c>
       <c r="K43" s="4"/>
       <c r="M43" s="44"/>
@@ -2219,11 +6258,11 @@
       <c r="B45" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="53">
+      <c r="C45" s="65">
         <f>J43</f>
-        <v>32180.275950604926</v>
-      </c>
-      <c r="D45" s="54"/>
+        <v>34541.334347611657</v>
+      </c>
+      <c r="D45" s="66"/>
       <c r="E45" s="15">
         <v>100</v>
       </c>
@@ -2239,10 +6278,10 @@
       <c r="B46" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="57">
+      <c r="C46" s="68">
         <v>28500</v>
       </c>
-      <c r="D46" s="58"/>
+      <c r="D46" s="69"/>
       <c r="E46" s="15"/>
       <c r="M46" s="44"/>
     </row>
@@ -2250,14 +6289,14 @@
       <c r="B47" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="57">
+      <c r="C47" s="68">
         <f>C46-C49-C50</f>
         <v>27075</v>
       </c>
-      <c r="D47" s="58"/>
+      <c r="D47" s="69"/>
       <c r="E47" s="15">
         <f>C47/C45*100</f>
-        <v>84.135387905183705</v>
+        <v>78.38434881387866</v>
       </c>
       <c r="M47" s="44"/>
     </row>
@@ -2265,14 +6304,14 @@
       <c r="B48" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="59">
+      <c r="C48" s="70">
         <f>C45-C47</f>
-        <v>5105.275950604926</v>
-      </c>
-      <c r="D48" s="59"/>
+        <v>7466.334347611657</v>
+      </c>
+      <c r="D48" s="70"/>
       <c r="E48" s="15">
         <f>100-E47</f>
-        <v>15.864612094816295</v>
+        <v>21.61565118612134</v>
       </c>
       <c r="M48" s="44"/>
     </row>
@@ -2280,11 +6319,11 @@
       <c r="B49" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C49" s="53">
+      <c r="C49" s="65">
         <f>C46*0.03</f>
         <v>855</v>
       </c>
-      <c r="D49" s="54"/>
+      <c r="D49" s="66"/>
       <c r="E49" s="15">
         <v>3</v>
       </c>
@@ -2294,11 +6333,11 @@
       <c r="B50" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="53">
+      <c r="C50" s="65">
         <f>C46*0.02</f>
         <v>570</v>
       </c>
-      <c r="D50" s="54"/>
+      <c r="D50" s="66"/>
       <c r="E50" s="15">
         <v>2</v>
       </c>
@@ -2306,13 +6345,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C49:D49"/>
     <mergeCell ref="C50:D50"/>
     <mergeCell ref="A7:F7"/>
@@ -2321,6 +6353,13 @@
     <mergeCell ref="C46:D46"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2334,7 +6373,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
@@ -2358,34 +6397,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
+      <c r="B2" s="74"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
@@ -2418,30 +6457,30 @@
       <c r="K4" s="63"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="76"/>
-      <c r="K5" s="76"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="72" t="e">
+      <c r="C6" s="71" t="e">
         <f>F30</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="73"/>
+      <c r="D6" s="72"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -2449,11 +6488,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="11"/>
-      <c r="J6" s="72" t="e">
+      <c r="J6" s="71" t="e">
         <f>I30</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="73"/>
+      <c r="K6" s="72"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
@@ -2462,77 +6501,77 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="I7" s="69" t="s">
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="I7" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="e">
+      <c r="A8" s="78" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="I8" s="70" t="s">
+      <c r="B8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="I8" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="67" t="e">
+      <c r="A9" s="78" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="I9" s="70" t="s">
+      <c r="B9" s="78"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="I9" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="65" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="66" t="s">
+      <c r="K11" s="77" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="14" t="s">
         <v>26</v>
       </c>
@@ -2551,8 +6590,8 @@
       <c r="I12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="65"/>
-      <c r="K12" s="66"/>
+      <c r="J12" s="76"/>
+      <c r="K12" s="77"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
@@ -3065,13 +7104,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -3085,6 +7117,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>